<commit_message>
more package 12 updates
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_FT_6MWT.xlsx
+++ b/curation/draft/collection/collection_specialization_FT_6MWT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD62E31-070A-423C-88A7-D59C2912A4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEE8A7E-0F7D-45E2-8201-24B5F7405917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_FT!$A$1:$AG$17</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="126">
   <si>
     <t>package_date</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>FTSTAT</t>
+  </si>
+  <si>
+    <t>C115409</t>
   </si>
 </sst>
 </file>
@@ -778,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1111,7 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>33</v>

</xml_diff>